<commit_message>
vault backup: 2023-03-08 11:41:27
</commit_message>
<xml_diff>
--- a/Algorithms/Logistic_Regression/Sigmoid Function shape.xlsx
+++ b/Algorithms/Logistic_Regression/Sigmoid Function shape.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\A000 Next Step\B10-ML\A00-ML\0  Oracle ML\Day3\Logistic_Regression\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TASUMANT\personal\DSandML\Algorithms\Logistic_Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4EA891A-90D9-486D-A323-BE027E3EF630}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E191390-6E23-4D81-9EB5-5532B5C98188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1D319D35-9FA3-4F4E-B4DD-3FC542EC14EE}"/>
+    <workbookView xWindow="-28920" yWindow="-2925" windowWidth="29040" windowHeight="17520" xr2:uid="{1D319D35-9FA3-4F4E-B4DD-3FC542EC14EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1822,23 +1822,23 @@
   <dimension ref="B1:F83"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.109375" customWidth="1"/>
-    <col min="2" max="3" width="8.44140625" customWidth="1"/>
-    <col min="4" max="4" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="2" max="3" width="8.42578125" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
@@ -1855,7 +1855,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="6">
         <v>0</v>
       </c>
@@ -1874,7 +1874,7 @@
         <v>4.5397868702434395E-5</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D4" s="1">
         <v>-19.5</v>
       </c>
@@ -1887,7 +1887,7 @@
         <v>5.8291265661138651E-5</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D5" s="1">
         <v>-19</v>
       </c>
@@ -1900,7 +1900,7 @@
         <v>7.4846227510611229E-5</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D6" s="1">
         <v>-18.5</v>
       </c>
@@ -1913,7 +1913,7 @@
         <v>9.6102415499473961E-5</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D7" s="1">
         <v>-18</v>
       </c>
@@ -1926,7 +1926,7 @@
         <v>1.2339457598623172E-4</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D8" s="1">
         <v>-17.5</v>
       </c>
@@ -1939,7 +1939,7 @@
         <v>1.5843621910252592E-4</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D9" s="1">
         <v>-17</v>
       </c>
@@ -1952,7 +1952,7 @@
         <v>2.0342697805520653E-4</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D10" s="1">
         <v>-16.5</v>
       </c>
@@ -1965,7 +1965,7 @@
         <v>2.6119031909571942E-4</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D11" s="1">
         <v>-16</v>
       </c>
@@ -1978,7 +1978,7 @@
         <v>3.3535013046647811E-4</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D12" s="1">
         <v>-15.5</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v>4.3055708132461488E-4</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D13" s="1">
         <v>-15</v>
       </c>
@@ -2004,7 +2004,7 @@
         <v>5.5277863692359955E-4</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D14" s="1">
         <v>-14.5</v>
       </c>
@@ -2017,7 +2017,7 @@
         <v>7.0967039910058811E-4</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D15" s="1">
         <v>-14</v>
       </c>
@@ -2030,7 +2030,7 @@
         <v>9.1105119440064539E-4</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D16" s="1">
         <v>-13.5</v>
       </c>
@@ -2043,7 +2043,7 @@
         <v>1.1695102650555148E-3</v>
       </c>
     </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D17" s="1">
         <v>-13</v>
       </c>
@@ -2056,7 +2056,7 @@
         <v>1.5011822567369917E-3</v>
       </c>
     </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D18" s="1">
         <v>-12.5</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>1.9267346633274757E-3</v>
       </c>
     </row>
-    <row r="19" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D19" s="1">
         <v>-12</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>2.4726231566347743E-3</v>
       </c>
     </row>
-    <row r="20" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D20" s="1">
         <v>-11.5</v>
       </c>
@@ -2095,7 +2095,7 @@
         <v>3.1726828424851893E-3</v>
       </c>
     </row>
-    <row r="21" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D21" s="1">
         <v>-11</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>4.0701377158961277E-3</v>
       </c>
     </row>
-    <row r="22" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D22" s="1">
         <v>-10.5</v>
       </c>
@@ -2121,7 +2121,7 @@
         <v>5.2201256935583973E-3</v>
       </c>
     </row>
-    <row r="23" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D23" s="1">
         <v>-10</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>6.6928509242848554E-3</v>
       </c>
     </row>
-    <row r="24" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D24" s="1">
         <v>-9.5</v>
       </c>
@@ -2147,7 +2147,7 @@
         <v>8.5774854137119841E-3</v>
       </c>
     </row>
-    <row r="25" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D25" s="1">
         <v>-9</v>
       </c>
@@ -2160,7 +2160,7 @@
         <v>1.098694263059318E-2</v>
       </c>
     </row>
-    <row r="26" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D26" s="1">
         <v>-8.5</v>
       </c>
@@ -2173,7 +2173,7 @@
         <v>1.4063627043245475E-2</v>
       </c>
     </row>
-    <row r="27" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D27" s="1">
         <v>-8</v>
       </c>
@@ -2186,7 +2186,7 @@
         <v>1.7986209962091559E-2</v>
       </c>
     </row>
-    <row r="28" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D28" s="1">
         <v>-7.5</v>
       </c>
@@ -2199,7 +2199,7 @@
         <v>2.2977369910025615E-2</v>
       </c>
     </row>
-    <row r="29" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D29" s="1">
         <v>-7</v>
       </c>
@@ -2212,7 +2212,7 @@
         <v>2.9312230751356319E-2</v>
       </c>
     </row>
-    <row r="30" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D30" s="1">
         <v>-6.5</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>3.7326887344129457E-2</v>
       </c>
     </row>
-    <row r="31" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D31" s="1">
         <v>-6</v>
       </c>
@@ -2238,7 +2238,7 @@
         <v>4.7425873177566781E-2</v>
       </c>
     </row>
-    <row r="32" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D32" s="1">
         <v>-5.5</v>
       </c>
@@ -2251,7 +2251,7 @@
         <v>6.0086650174007626E-2</v>
       </c>
     </row>
-    <row r="33" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D33" s="1">
         <v>-5</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>7.5858180021243546E-2</v>
       </c>
     </row>
-    <row r="34" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D34" s="1">
         <v>-4.5</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>9.534946489910949E-2</v>
       </c>
     </row>
-    <row r="35" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D35" s="1">
         <v>-4</v>
       </c>
@@ -2290,7 +2290,7 @@
         <v>0.11920292202211755</v>
       </c>
     </row>
-    <row r="36" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D36" s="1">
         <v>-3.5</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>0.14804719803168948</v>
       </c>
     </row>
-    <row r="37" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D37" s="1">
         <v>-3</v>
       </c>
@@ -2316,7 +2316,7 @@
         <v>0.18242552380635635</v>
       </c>
     </row>
-    <row r="38" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D38" s="1">
         <v>-2.5</v>
       </c>
@@ -2329,7 +2329,7 @@
         <v>0.22270013882530884</v>
       </c>
     </row>
-    <row r="39" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D39" s="1">
         <v>-2</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>0.2689414213699951</v>
       </c>
     </row>
-    <row r="40" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D40" s="1">
         <v>-1.5</v>
       </c>
@@ -2355,7 +2355,7 @@
         <v>0.32082130082460703</v>
       </c>
     </row>
-    <row r="41" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D41" s="1">
         <v>-1</v>
       </c>
@@ -2368,7 +2368,7 @@
         <v>0.37754066879814541</v>
       </c>
     </row>
-    <row r="42" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D42" s="1">
         <v>-0.5</v>
       </c>
@@ -2381,7 +2381,7 @@
         <v>0.43782349911420193</v>
       </c>
     </row>
-    <row r="43" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D43" s="1">
         <v>0</v>
       </c>
@@ -2394,7 +2394,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="44" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D44" s="1">
         <v>0.5</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>0.56217650088579807</v>
       </c>
     </row>
-    <row r="45" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D45" s="1">
         <v>1</v>
       </c>
@@ -2420,7 +2420,7 @@
         <v>0.62245933120185459</v>
       </c>
     </row>
-    <row r="46" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D46" s="1">
         <v>1.5</v>
       </c>
@@ -2433,7 +2433,7 @@
         <v>0.67917869917539297</v>
       </c>
     </row>
-    <row r="47" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D47" s="1">
         <v>2</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>0.7310585786300049</v>
       </c>
     </row>
-    <row r="48" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D48" s="1">
         <v>2.5</v>
       </c>
@@ -2459,7 +2459,7 @@
         <v>0.77729986117469108</v>
       </c>
     </row>
-    <row r="49" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D49" s="1">
         <v>3</v>
       </c>
@@ -2472,7 +2472,7 @@
         <v>0.81757447619364365</v>
       </c>
     </row>
-    <row r="50" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D50" s="1">
         <v>3.5</v>
       </c>
@@ -2485,7 +2485,7 @@
         <v>0.85195280196831058</v>
       </c>
     </row>
-    <row r="51" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D51" s="1">
         <v>4</v>
       </c>
@@ -2498,7 +2498,7 @@
         <v>0.88079707797788231</v>
       </c>
     </row>
-    <row r="52" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D52" s="1">
         <v>4.5</v>
       </c>
@@ -2511,7 +2511,7 @@
         <v>0.90465053510089055</v>
       </c>
     </row>
-    <row r="53" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D53" s="1">
         <v>5</v>
       </c>
@@ -2524,7 +2524,7 @@
         <v>0.92414181997875655</v>
       </c>
     </row>
-    <row r="54" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D54" s="1">
         <v>5.5</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>0.93991334982599239</v>
       </c>
     </row>
-    <row r="55" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D55" s="1">
         <v>6</v>
       </c>
@@ -2550,7 +2550,7 @@
         <v>0.95257412682243336</v>
       </c>
     </row>
-    <row r="56" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D56" s="1">
         <v>6.5</v>
       </c>
@@ -2563,7 +2563,7 @@
         <v>0.96267311265587063</v>
       </c>
     </row>
-    <row r="57" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D57" s="1">
         <v>7</v>
       </c>
@@ -2576,7 +2576,7 @@
         <v>0.97068776924864364</v>
       </c>
     </row>
-    <row r="58" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D58" s="1">
         <v>7.5</v>
       </c>
@@ -2589,7 +2589,7 @@
         <v>0.97702263008997436</v>
       </c>
     </row>
-    <row r="59" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D59" s="1">
         <v>8</v>
       </c>
@@ -2602,7 +2602,7 @@
         <v>0.98201379003790845</v>
       </c>
     </row>
-    <row r="60" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D60" s="1">
         <v>8.5</v>
       </c>
@@ -2615,7 +2615,7 @@
         <v>0.9859363729567544</v>
       </c>
     </row>
-    <row r="61" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D61" s="1">
         <v>9</v>
       </c>
@@ -2628,7 +2628,7 @@
         <v>0.98901305736940681</v>
       </c>
     </row>
-    <row r="62" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D62" s="1">
         <v>9.5</v>
       </c>
@@ -2641,7 +2641,7 @@
         <v>0.99142251458628805</v>
       </c>
     </row>
-    <row r="63" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D63" s="1">
         <v>10</v>
       </c>
@@ -2654,7 +2654,7 @@
         <v>0.99330714907571527</v>
       </c>
     </row>
-    <row r="64" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D64" s="1">
         <v>10.5</v>
       </c>
@@ -2667,7 +2667,7 @@
         <v>0.99477987430644166</v>
       </c>
     </row>
-    <row r="65" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D65" s="1">
         <v>11</v>
       </c>
@@ -2680,7 +2680,7 @@
         <v>0.99592986228410396</v>
       </c>
     </row>
-    <row r="66" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D66" s="1">
         <v>11.5</v>
       </c>
@@ -2693,7 +2693,7 @@
         <v>0.99682731715751483</v>
       </c>
     </row>
-    <row r="67" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D67" s="1">
         <v>12</v>
       </c>
@@ -2706,7 +2706,7 @@
         <v>0.99752737684336534</v>
       </c>
     </row>
-    <row r="68" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D68" s="1">
         <v>12.5</v>
       </c>
@@ -2719,7 +2719,7 @@
         <v>0.99807326533667251</v>
       </c>
     </row>
-    <row r="69" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D69" s="1">
         <v>13</v>
       </c>
@@ -2732,7 +2732,7 @@
         <v>0.99849881774326299</v>
       </c>
     </row>
-    <row r="70" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D70" s="1">
         <v>13.5</v>
       </c>
@@ -2745,7 +2745,7 @@
         <v>0.99883048973494448</v>
       </c>
     </row>
-    <row r="71" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D71" s="1">
         <v>14</v>
       </c>
@@ -2758,7 +2758,7 @@
         <v>0.9990889488055994</v>
       </c>
     </row>
-    <row r="72" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D72" s="1">
         <v>14.5</v>
       </c>
@@ -2771,7 +2771,7 @@
         <v>0.99929032960089947</v>
       </c>
     </row>
-    <row r="73" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D73" s="1">
         <v>15</v>
       </c>
@@ -2784,7 +2784,7 @@
         <v>0.9994472213630764</v>
       </c>
     </row>
-    <row r="74" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D74" s="1">
         <v>15.5</v>
       </c>
@@ -2797,7 +2797,7 @@
         <v>0.99956944291867544</v>
       </c>
     </row>
-    <row r="75" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D75" s="1">
         <v>16</v>
       </c>
@@ -2810,7 +2810,7 @@
         <v>0.99966464986953363</v>
       </c>
     </row>
-    <row r="76" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D76" s="1">
         <v>16.5</v>
       </c>
@@ -2823,7 +2823,7 @@
         <v>0.99973880968090434</v>
       </c>
     </row>
-    <row r="77" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D77" s="1">
         <v>17</v>
       </c>
@@ -2836,7 +2836,7 @@
         <v>0.9997965730219448</v>
       </c>
     </row>
-    <row r="78" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D78" s="1">
         <v>17.5</v>
       </c>
@@ -2849,7 +2849,7 @@
         <v>0.9998415637808975</v>
       </c>
     </row>
-    <row r="79" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D79" s="1">
         <v>18</v>
       </c>
@@ -2862,7 +2862,7 @@
         <v>0.99987660542401369</v>
       </c>
     </row>
-    <row r="80" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D80" s="1">
         <v>18.5</v>
       </c>
@@ -2875,7 +2875,7 @@
         <v>0.99990389758450049</v>
       </c>
     </row>
-    <row r="81" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D81" s="1">
         <v>19</v>
       </c>
@@ -2888,7 +2888,7 @@
         <v>0.99992515377248947</v>
       </c>
     </row>
-    <row r="82" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D82" s="1">
         <v>19.5</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>0.99994170873433885</v>
       </c>
     </row>
-    <row r="83" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D83" s="1">
         <v>20</v>
       </c>

</xml_diff>